<commit_message>
update for  order audit and note audit
</commit_message>
<xml_diff>
--- a/resources/admissionCreatePatient.xlsx
+++ b/resources/admissionCreatePatient.xlsx
@@ -482,7 +482,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C13"/>
+      <selection activeCell="C6" sqref="C6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1"/>
@@ -495,7 +495,7 @@
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1">
+    <row r="1" spans="1:8" ht="56.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="15">
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Update Special Orders , Discharge Address Primary Care Giver
</commit_message>
<xml_diff>
--- a/resources/admissionCreatePatient.xlsx
+++ b/resources/admissionCreatePatient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -114,9 +114,6 @@
     <t>//md-select[@ng-model="vm.newpatient.gender"]</t>
   </si>
   <si>
-    <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]/md-select-menu/md-content/md-option[1]</t>
-  </si>
-  <si>
     <t>//md-datepicker[@ng-model="vm.newpatient.birthday"]/div[1]/input</t>
   </si>
   <si>
@@ -135,28 +132,76 @@
     <t>/html/body/div[1]/div/md-content/div/section/div[1]/button</t>
   </si>
   <si>
-    <t>/html/body/div[1]/div/md-content/md-content/md-content[3]/md-content/div/div/div/div[1]/button[2]</t>
-  </si>
-  <si>
-    <t>//*[@id="dialogContent_15"]</t>
-  </si>
-  <si>
-    <t>Medicaid Number</t>
-  </si>
-  <si>
-    <t>//input[@ng-model="vm.newpatient.mrnNumber"]</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>HIC number</t>
-  </si>
-  <si>
-    <t>//input[@ng-model="vm.newpatient.hicNumber"]</t>
-  </si>
-  <si>
-    <t>412333</t>
+    <t>Add Button</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="vm.addOnePatientNumber()"]</t>
+  </si>
+  <si>
+    <t>HIC DropDown</t>
+  </si>
+  <si>
+    <t>//md-dialog[@class="mobile-fullwidth-dialog _md md-cs-content-theme-theme flex-md-80 flex-gt-md-60 flex-100 _md-transition-in"]</t>
+  </si>
+  <si>
+    <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[1]</t>
+  </si>
+  <si>
+    <t>//md-input-container[@class="md-block md-cs-content-theme-theme flex md-input-has-value"]</t>
+  </si>
+  <si>
+    <t>Med Num</t>
+  </si>
+  <si>
+    <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[2]</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>0015</t>
+  </si>
+  <si>
+    <t>//input[@ng-model="patientNumber.number"]</t>
+  </si>
+  <si>
+    <t>Add Button2</t>
+  </si>
+  <si>
+    <t>Number2</t>
+  </si>
+  <si>
+    <t>(//input[@ng-model="patientNumber.number"])[2]</t>
+  </si>
+  <si>
+    <t>Add Button3</t>
+  </si>
+  <si>
+    <t>Number3</t>
+  </si>
+  <si>
+    <t>(//input[@ng-model="patientNumber.number"])[3]</t>
+  </si>
+  <si>
+    <t>0016</t>
+  </si>
+  <si>
+    <t>0017</t>
+  </si>
+  <si>
+    <t>Searchbtn</t>
+  </si>
+  <si>
+    <t>Searchtxtbox</t>
+  </si>
+  <si>
+    <t>//input[@ng-model="vm.patientSearch"]</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="vm.filterShow = false"]</t>
+  </si>
+  <si>
+    <t>//button[@ng-show="vm.admissionKeys.length &lt;= 1000 &amp;&amp; vm.admissionStatus =='All'"]</t>
   </si>
 </sst>
 </file>
@@ -497,19 +542,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="37.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" style="3" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="20.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -539,12 +584,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="15">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -560,12 +605,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="15">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -586,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -602,12 +647,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="15">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="45">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -719,12 +764,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="45">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -745,7 +790,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -765,38 +810,52 @@
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="15">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="15">
-      <c r="A13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>8</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="30">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
@@ -812,15 +871,194 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1">
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="15">
       <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="15">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="1" customFormat="1" ht="15">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="15">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" ht="15">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="21" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="21" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>